<commit_message>
feat(link-import): change worksheet format
</commit_message>
<xml_diff>
--- a/Link导入样表.xlsx
+++ b/Link导入样表.xlsx
@@ -16,18 +16,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>镜头</t>
   </si>
   <si>
-    <t>资产</t>
+    <t>资产1</t>
+  </si>
+  <si>
+    <t>资产2</t>
   </si>
   <si>
     <t>SDKTEST_EP01_01_sc001</t>
   </si>
   <si>
     <t>asset1</t>
+  </si>
+  <si>
+    <t>asset2</t>
+  </si>
+  <si>
+    <t>SDKTEST_EP01_01_sc002</t>
+  </si>
+  <si>
+    <t>SDKTEST_EP01_01_sc003</t>
   </si>
 </sst>
 </file>
@@ -171,23 +183,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,6 +220,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -220,30 +256,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -256,48 +268,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -316,6 +328,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -328,7 +376,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,48 +395,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,10 +513,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -513,115 +525,115 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -630,13 +642,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -995,31 +1007,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>